<commit_message>
Added a document showing FixAlign participant numbering changes.
</commit_message>
<xml_diff>
--- a/FixAlign/FA_analysis/Actual Participant numbers.xlsx
+++ b/FixAlign/FA_analysis/Actual Participant numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethle-luan/Desktop/Duncans_Grant/FixAlign/FA_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliza\Desktop\Duncans_Grant\FixAlign\FA_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6E6B59-71B5-E044-B6DD-78FE61FC8545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A703FBB-363C-484A-BD09-2384DB6B64FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1220" windowWidth="25040" windowHeight="13680" xr2:uid="{5753FD6A-6C0C-AC46-901B-72DB17396E19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753FD6A-6C0C-AC46-901B-72DB17396E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Participant R_corr</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Actual # on IDs</t>
+  </si>
+  <si>
+    <t>Lost participants due to FixAlign problems</t>
   </si>
 </sst>
 </file>
@@ -388,20 +391,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2481237-A351-5342-AA63-73152964A451}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +418,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -428,8 +435,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -442,8 +452,11 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -456,8 +469,11 @@
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -470,8 +486,11 @@
       <c r="D5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -484,8 +503,11 @@
       <c r="D6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -499,7 +521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -513,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -527,7 +549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -541,7 +563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -555,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -569,7 +591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -583,7 +605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -597,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -611,7 +633,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -625,7 +647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -639,7 +661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -653,7 +675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -667,7 +689,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -681,7 +703,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -695,7 +717,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -709,7 +731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -723,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -737,7 +759,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -751,7 +773,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -765,7 +787,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -779,7 +801,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -793,7 +815,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -807,7 +829,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -821,7 +843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -829,7 +851,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -837,7 +859,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -845,7 +867,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -853,7 +875,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -861,7 +883,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -869,7 +891,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -877,7 +899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -885,7 +907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -893,7 +915,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -901,7 +923,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -909,7 +931,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -917,7 +939,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -925,7 +947,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -933,7 +955,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -941,7 +963,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -949,7 +971,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -957,7 +979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -965,7 +987,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -973,7 +995,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -981,7 +1003,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>

</xml_diff>